<commit_message>
Code Main V2.1.2 Upload
</commit_message>
<xml_diff>
--- a/Scraped Data/Escorp Asset Management Ltd_Data.xlsx
+++ b/Scraped Data/Escorp Asset Management Ltd_Data.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="29">
   <si>
     <t>Mar 2016</t>
   </si>
@@ -34,6 +34,33 @@
     <t>Debts</t>
   </si>
   <si>
+    <t>Cash</t>
+  </si>
+  <si>
+    <t>Cash Eq</t>
+  </si>
+  <si>
+    <t>0.00</t>
+  </si>
+  <si>
+    <t>Mar 2017</t>
+  </si>
+  <si>
+    <t>2.65</t>
+  </si>
+  <si>
+    <t>Mar 2018</t>
+  </si>
+  <si>
+    <t>Mar 2019</t>
+  </si>
+  <si>
+    <t>Mar 2020</t>
+  </si>
+  <si>
+    <t>Mar 2021</t>
+  </si>
+  <si>
     <t>Total</t>
   </si>
   <si>
@@ -46,52 +73,34 @@
     <t>PAT</t>
   </si>
   <si>
-    <t>Cash</t>
-  </si>
-  <si>
-    <t>Cash Eq</t>
-  </si>
-  <si>
-    <t>0.00</t>
-  </si>
-  <si>
-    <t>Mar 2017</t>
-  </si>
-  <si>
-    <t>2.65</t>
-  </si>
-  <si>
     <t>0.22</t>
   </si>
   <si>
     <t>0.18</t>
   </si>
   <si>
-    <t>Mar 2018</t>
-  </si>
-  <si>
     <t>0.10</t>
   </si>
   <si>
     <t>0.08</t>
   </si>
   <si>
-    <t>Mar 2019</t>
-  </si>
-  <si>
     <t>-0.08</t>
   </si>
   <si>
-    <t>Mar 2020</t>
-  </si>
-  <si>
     <t>0.01</t>
   </si>
   <si>
-    <t>Mar 2021</t>
-  </si>
-  <si>
     <t>0.02</t>
+  </si>
+  <si>
+    <t>Mar 2022</t>
+  </si>
+  <si>
+    <t>6.17</t>
+  </si>
+  <si>
+    <t>5.86</t>
   </si>
 </sst>
 </file>
@@ -445,7 +454,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AK4"/>
+  <dimension ref="A1:AQ4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -470,9 +479,11 @@
     <col min="32" max="32" width="15.7109375" customWidth="1"/>
     <col min="34" max="34" width="15.7109375" customWidth="1"/>
     <col min="37" max="37" width="10.7109375" customWidth="1"/>
+    <col min="40" max="40" width="15.7109375" customWidth="1"/>
+    <col min="43" max="43" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:37">
+    <row r="1" spans="1:43">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -482,7 +493,7 @@
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
       <c r="H1" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
@@ -490,7 +501,7 @@
       <c r="L1" s="1"/>
       <c r="M1" s="1"/>
       <c r="N1" s="1" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="O1" s="1"/>
       <c r="P1" s="1"/>
@@ -498,7 +509,7 @@
       <c r="R1" s="1"/>
       <c r="S1" s="1"/>
       <c r="T1" s="1" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="U1" s="1"/>
       <c r="V1" s="1"/>
@@ -506,7 +517,7 @@
       <c r="X1" s="1"/>
       <c r="Y1" s="1"/>
       <c r="Z1" s="1" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="AA1" s="1"/>
       <c r="AB1" s="1"/>
@@ -514,15 +525,23 @@
       <c r="AD1" s="1"/>
       <c r="AE1" s="1"/>
       <c r="AF1" s="1" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="AG1" s="1"/>
       <c r="AH1" s="1"/>
       <c r="AI1" s="1"/>
       <c r="AJ1" s="1"/>
       <c r="AK1" s="1"/>
+      <c r="AL1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AM1" s="1"/>
+      <c r="AN1" s="1"/>
+      <c r="AO1" s="1"/>
+      <c r="AP1" s="1"/>
+      <c r="AQ1" s="1"/>
     </row>
-    <row r="2" spans="1:37">
+    <row r="2" spans="1:43">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -533,16 +552,16 @@
         <v>5</v>
       </c>
       <c r="D2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G2" s="2" t="s">
         <v>6</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>10</v>
       </c>
       <c r="H2" s="2" t="s">
         <v>3</v>
@@ -551,16 +570,16 @@
         <v>5</v>
       </c>
       <c r="J2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="M2" s="2" t="s">
         <v>6</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="L2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="M2" s="2" t="s">
-        <v>10</v>
       </c>
       <c r="N2" s="2" t="s">
         <v>3</v>
@@ -569,16 +588,16 @@
         <v>5</v>
       </c>
       <c r="P2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="R2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="S2" s="2" t="s">
         <v>6</v>
-      </c>
-      <c r="Q2" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="R2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="S2" s="2" t="s">
-        <v>10</v>
       </c>
       <c r="T2" s="2" t="s">
         <v>3</v>
@@ -587,16 +606,16 @@
         <v>5</v>
       </c>
       <c r="V2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="W2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="X2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="Y2" s="2" t="s">
         <v>6</v>
-      </c>
-      <c r="W2" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="X2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="Y2" s="2" t="s">
-        <v>10</v>
       </c>
       <c r="Z2" s="2" t="s">
         <v>3</v>
@@ -605,16 +624,16 @@
         <v>5</v>
       </c>
       <c r="AB2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="AC2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="AD2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="AE2" s="2" t="s">
         <v>6</v>
-      </c>
-      <c r="AC2" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="AD2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="AE2" s="2" t="s">
-        <v>10</v>
       </c>
       <c r="AF2" s="2" t="s">
         <v>3</v>
@@ -623,75 +642,93 @@
         <v>5</v>
       </c>
       <c r="AH2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="AI2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="AJ2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="AK2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="AI2" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="AJ2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="AK2" s="2" t="s">
-        <v>10</v>
+      <c r="AN2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="AO2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="AP2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="AQ2" s="2" t="s">
+        <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:37">
+    <row r="3" spans="1:43">
       <c r="B3" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D3" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G3" s="2" t="s">
         <v>7</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>11</v>
       </c>
       <c r="H3" s="2" t="s">
         <v>4</v>
       </c>
       <c r="J3" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="M3" s="2" t="s">
         <v>7</v>
-      </c>
-      <c r="M3" s="2" t="s">
-        <v>11</v>
       </c>
       <c r="N3" s="2" t="s">
         <v>4</v>
       </c>
       <c r="P3" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="S3" s="2" t="s">
         <v>7</v>
-      </c>
-      <c r="S3" s="2" t="s">
-        <v>11</v>
       </c>
       <c r="T3" s="2" t="s">
         <v>4</v>
       </c>
       <c r="V3" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="Y3" s="2" t="s">
         <v>7</v>
-      </c>
-      <c r="Y3" s="2" t="s">
-        <v>11</v>
       </c>
       <c r="Z3" s="2" t="s">
         <v>4</v>
       </c>
       <c r="AB3" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="AE3" s="2" t="s">
         <v>7</v>
-      </c>
-      <c r="AE3" s="2" t="s">
-        <v>11</v>
       </c>
       <c r="AF3" s="2" t="s">
         <v>4</v>
       </c>
       <c r="AH3" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="AK3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="AK3" s="2" t="s">
-        <v>11</v>
+      <c r="AN3" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="AQ3" s="2" t="s">
+        <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:37">
+    <row r="4" spans="1:43">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
@@ -699,82 +736,82 @@
         <v>0.01</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D4" s="2">
         <v>0</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="H4" s="2">
         <v>8.309999999999999</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="J4" s="2">
         <v>0.51</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="L4" s="2" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="N4" s="2">
         <v>14.82</v>
       </c>
       <c r="O4" s="2" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="P4" s="2">
         <v>0.29</v>
       </c>
       <c r="Q4" s="2" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="R4" s="2" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="T4" s="2">
         <v>15.4</v>
       </c>
       <c r="U4" s="2" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="V4" s="2">
         <v>0.25</v>
       </c>
       <c r="W4" s="2" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="X4" s="2" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="Z4" s="2">
         <v>15.32</v>
       </c>
       <c r="AA4" s="2" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="AB4" s="2">
         <v>0.16</v>
       </c>
       <c r="AC4" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="AD4" s="2" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="AF4" s="2">
         <v>24.66</v>
       </c>
       <c r="AG4" s="2" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="AH4" s="2">
         <v>0.17</v>
@@ -783,11 +820,20 @@
         <v>25</v>
       </c>
       <c r="AJ4" s="2" t="s">
-        <v>12</v>
+        <v>8</v>
+      </c>
+      <c r="AN4" s="2">
+        <v>6.33</v>
+      </c>
+      <c r="AO4" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="AP4" s="2" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="14">
     <mergeCell ref="B1:G1"/>
     <mergeCell ref="B1:G1"/>
     <mergeCell ref="H1:M1"/>
@@ -795,6 +841,13 @@
     <mergeCell ref="T1:Y1"/>
     <mergeCell ref="Z1:AE1"/>
     <mergeCell ref="AF1:AK1"/>
+    <mergeCell ref="B1:G1"/>
+    <mergeCell ref="H1:M1"/>
+    <mergeCell ref="N1:S1"/>
+    <mergeCell ref="T1:Y1"/>
+    <mergeCell ref="Z1:AE1"/>
+    <mergeCell ref="AF1:AK1"/>
+    <mergeCell ref="AL1:AQ1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>